<commit_message>
update discord account and task evidence
</commit_message>
<xml_diff>
--- a/dee-effes/evidence.xlsx
+++ b/dee-effes/evidence.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26307"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BC89DD6-7A3C-4694-AF9B-AB721A97F36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31235FB9-CDD3-4797-84F3-612DE01679FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>omniflix106lu2m62qk83v0j3tvw7053yjrkqqlnz4kurmh</t>
   </si>
   <si>
-    <t>Pippin Ain't Easy#0669</t>
+    <t>GameOfNFTs | blockscape#1151</t>
   </si>
   <si>
     <t>none</t>
@@ -483,7 +483,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update evidence for dee-effes
</commit_message>
<xml_diff>
--- a/dee-effes/evidence.xlsx
+++ b/dee-effes/evidence.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31235FB9-CDD3-4797-84F3-612DE01679FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBA96ABB-F2CE-48D4-808B-0C9F2B96FFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>TeamName</t>
   </si>
@@ -90,37 +90,55 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>5E0341B26070B851A9179F1660D4DD5CCAA551EF9336BCA227734B5D9F8685B6</t>
-  </si>
-  <si>
-    <t>blcsClass</t>
+    <t>444971A9CE8D7F91F05F790791C437569F7920C73B0860D7FA481A53DC26B6CB</t>
+  </si>
+  <si>
+    <t>blcsBenni001</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>3FE7E893F9DA60CCE309D9A951343698D11E275501F8A691F64CA62B303D0E03</t>
-  </si>
-  <si>
-    <t>blcsNFTgregy001</t>
-  </si>
-  <si>
-    <t>B3F292FF3EFD8345D79754BF7C59ED2B89C2CD091CC33451E594B50FE1489629</t>
-  </si>
-  <si>
-    <t>blcsNFTbenko001</t>
+    <t>81C700D246F57039F3BDC16B0DA0C7CFF937356271269FD8CF50A87316923F9D</t>
+  </si>
+  <si>
+    <t>blcsNFTBenni002</t>
+  </si>
+  <si>
+    <t>4AED26214C9A72F97E381AEB3385199F14BDA6324448FAB0029202D092C80018</t>
+  </si>
+  <si>
+    <t>blcsNFTmars001</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>C7ED2517C6BCC27D42FBC337D3F6EDF7BC5B53E1801EB2C218E0B78C712D4EA6</t>
-  </si>
-  <si>
-    <t>stars1qex20hgqvv4swrhdgxj8lt2da3g726xprutc7q9lhuwltsw59ptshtqty6</t>
+    <t>5F0E44A16797DD129730B38EFA84F240C3D8EA8A82384DBBB7BFBDCA2AA4B916</t>
+  </si>
+  <si>
+    <t>stars1yxv9njz6nfpwxtxzfawe5a2mv7z9gu9hl23zhu7g5c4jaxh7y4nqjkav4n</t>
   </si>
   <si>
     <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>1A0C443A20A619C1DE7858139C0B13FA77A4CFA463D7AF035C67A65B5FD318E1</t>
+  </si>
+  <si>
+    <t>ibc/6EAF424647FC10605DA6FFF50CF3FD26D3AA49495FA211FE0551F84DD9E79C7F</t>
+  </si>
+  <si>
+    <t>blcsNFTBenni005</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>B1FC2856C78D496EE0F4541EA15FCE2DAC5D630E2C8047C59A27CB02726241BA</t>
+  </si>
+  <si>
+    <t>EA84CC14BE7E279EC05193B3FDD6FBBBB55702D16BF654C7EBA6E6D6CF7AA736</t>
   </si>
 </sst>
 </file>
@@ -482,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -560,7 +578,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -594,12 +612,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="72.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -646,7 +665,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,13 +710,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107752EB-189D-4603-881D-E5DB1965AE2D}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="71.42578125" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -713,6 +738,20 @@
         <v>25</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -720,13 +759,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BEB37F-1CAC-4981-B421-D7E70CDD6ADB}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="72" customWidth="1"/>
+    <col min="2" max="2" width="67.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -742,6 +786,20 @@
         <v>25</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -749,13 +807,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6814D2-7F01-4E99-BCAC-FCF637056EDF}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="73" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -771,6 +835,20 @@
         <v>25</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>